<commit_message>
Laid Framework for Database Build
Need to reduce granularity of some lookup fields
</commit_message>
<xml_diff>
--- a/Code/Data/DataModel.xlsx
+++ b/Code/Data/DataModel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/286e2ff89c220aa4/Documents/University of Rochester/M2/DSCC483_DataScienceCapstone/URMCVenitaltorAllocation/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/286e2ff89c220aa4/Documents/University of Rochester/M2/DSCC483_DataScienceCapstone/URMCVenitaltorAllocation/Code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="81" documentId="8_{DB37FB98-B15B-4FA2-A8E9-DF84CFB93E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74DAFF65-0C8E-4DFE-BF99-1DF2BB220A0E}"/>
@@ -363,16 +363,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1982,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85080695-A573-40A9-8C39-01FF35E4824E}">
   <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2004,18 +2004,18 @@
   <sheetData>
     <row r="1" spans="2:12" ht="2.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="H2" s="8" t="s">
+      <c r="F2" s="11"/>
+      <c r="H2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -2076,10 +2076,10 @@
       <c r="I5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="11"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
@@ -2129,18 +2129,18 @@
     </row>
     <row r="8" spans="2:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="E9" s="10" t="s">
+      <c r="C9" s="9"/>
+      <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="H9" s="10" t="s">
+      <c r="F9" s="9"/>
+      <c r="H9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
@@ -2188,14 +2188,14 @@
         <v>32</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="H13" s="8" t="s">
+      <c r="F13" s="11"/>
+      <c r="H13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
@@ -2290,10 +2290,10 @@
       <c r="I18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="11"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
@@ -2302,10 +2302,10 @@
       <c r="C19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="11"/>
+      <c r="F19" s="9"/>
       <c r="H19" s="1" t="s">
         <v>27</v>
       </c>
@@ -2349,10 +2349,10 @@
     </row>
     <row r="22" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="11"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E24" s="6" t="s">
@@ -2372,6 +2372,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="K5:L5"/>
@@ -2379,12 +2385,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>